<commit_message>
Finalizing write-up and poster.
</commit_message>
<xml_diff>
--- a/results/Comparison Summary.xlsx
+++ b/results/Comparison Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c21645ff62eb64b3/Documents/CS/CS6364/Project/query-intent-classifier/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{255BB9A1-D482-4B37-8023-3EE5944DE244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0C86E49-DED5-424C-8546-3EF4ADA44938}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="8_{255BB9A1-D482-4B37-8023-3EE5944DE244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D0FA7D9-FBCD-481B-B3D0-B82BBC2DD0C2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="7" xr2:uid="{F0CFEFF8-1945-4CCF-AE0B-130C86417C10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F0CFEFF8-1945-4CCF-AE0B-130C86417C10}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Description" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="43">
   <si>
     <t>precision</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Intent Classification</t>
   </si>
   <si>
-    <t>RASA</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 34M</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
   </si>
   <si>
     <t>Personal assistant data with 7 intents. Includes entities. Examples: rate this current novel 1 stars"</t>
-  </si>
-  <si>
-    <t>CoNLL</t>
   </si>
   <si>
     <t>Y</t>
@@ -174,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 133M</t>
+  </si>
+  <si>
+    <t>IOB</t>
   </si>
 </sst>
 </file>
@@ -278,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -293,8 +290,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -309,23 +317,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,7 +1006,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RASA</c:v>
+                  <c:v>DIET</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2765,8 +2761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E1FA26-A712-43B9-BBBA-118E50C12153}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2779,100 +2775,100 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>17</v>
+        <v>42</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2885,8 +2881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7521C4CE-7B16-420F-8E5D-3BAA9CAC44AF}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2990,40 +2986,40 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <f>AVERAGE(ATIS!B10,benchmarking_data!B10,SNIPS!B10)</f>
+        <f>AVERAGE(ATIS!C10,benchmarking_data!C10,SNIPS!C10)</f>
         <v>0.94715406626298826</v>
       </c>
       <c r="C8" s="1">
-        <f>AVERAGE(ATIS!C10,benchmarking_data!C10,SNIPS!C10)</f>
+        <f>AVERAGE(ATIS!D10,benchmarking_data!D10,SNIPS!D10)</f>
         <v>0.95596265368190603</v>
       </c>
       <c r="D8" s="1">
-        <f>AVERAGE(ATIS!D10,benchmarking_data!D10,SNIPS!D10)</f>
+        <f>AVERAGE(ATIS!E10,benchmarking_data!E10,SNIPS!E10)</f>
         <v>0.95153578110816106</v>
       </c>
       <c r="E8" s="1">
-        <f>AVERAGE(ATIS!E10,benchmarking_data!E10,SNIPS!E10)</f>
+        <f>AVERAGE(ATIS!F10,benchmarking_data!F10,SNIPS!F10)</f>
         <v>0.97577829406396255</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <f>AVERAGE(ATIS!B11,benchmarking_data!B11,SNIPS!B11)</f>
+        <f>AVERAGE(ATIS!C11,benchmarking_data!C11,SNIPS!C11)</f>
         <v>0.74143357608360638</v>
       </c>
       <c r="C9" s="1">
-        <f>AVERAGE(ATIS!C11,benchmarking_data!C11,SNIPS!C11)</f>
+        <f>AVERAGE(ATIS!D11,benchmarking_data!D11,SNIPS!D11)</f>
         <v>0.81927246621987437</v>
       </c>
       <c r="D9" s="1">
-        <f>AVERAGE(ATIS!D11,benchmarking_data!D11,SNIPS!D11)</f>
+        <f>AVERAGE(ATIS!E11,benchmarking_data!E11,SNIPS!E11)</f>
         <v>0.77742717205007639</v>
       </c>
       <c r="E9" s="1">
-        <f>AVERAGE(ATIS!E11,benchmarking_data!E11,SNIPS!E11)</f>
+        <f>AVERAGE(ATIS!F11,benchmarking_data!F11,SNIPS!F11)</f>
         <v>0.90081847792143233</v>
       </c>
     </row>
@@ -3040,10 +3036,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6067AA1-4016-4948-91A0-D787ADC256B1}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B16"/>
+      <selection sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3058,15 +3054,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -3092,7 +3088,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3110,12 +3106,12 @@
       <c r="F3" s="1">
         <v>500</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="16">
         <v>0.97799999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3131,10 +3127,10 @@
       <c r="F4" s="1">
         <v>500</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3152,12 +3148,12 @@
       <c r="F5" s="1">
         <v>500</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="16">
         <v>0.96199999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3173,102 +3169,96 @@
       <c r="F6" s="1">
         <v>500</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="B8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>0.95924064768285799</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>0.96408529741863003</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>0.96165687097677</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>0.98740854177301296</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>0.93839953943580801</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>0.95377413692217605</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>0.94602437608821799</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>0.98088725232333795</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="G3:G4"/>
@@ -3284,7 +3274,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3331,7 +3321,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3349,12 +3339,12 @@
       <c r="F3" s="1">
         <v>1540</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="16">
         <v>0.88571428571428501</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3370,10 +3360,10 @@
       <c r="F4" s="1">
         <v>1540</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3391,12 +3381,12 @@
       <c r="F5" s="1">
         <v>1540</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="16">
         <v>0.90649350649350602</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3412,20 +3402,20 @@
       <c r="F6" s="1">
         <v>1540</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11"/>
+      <c r="A12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3433,7 +3423,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3454,7 +3444,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3503,7 +3493,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3521,12 +3511,12 @@
       <c r="F3" s="1">
         <v>1448</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="16">
         <v>0.99861878453038599</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3542,10 +3532,10 @@
       <c r="F4" s="1">
         <v>1448</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3563,12 +3553,12 @@
       <c r="F5" s="1">
         <v>1448</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="16">
         <v>0.98618784530386705</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3584,80 +3574,80 @@
       <c r="F6" s="1">
         <v>1448</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="B8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>0.93860404997845703</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>0.94985829518203602</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>0.94419763788059297</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>0.97037820682359099</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>0.64900514196288805</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>0.77661851257356795</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>0.70710023139690603</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>0.87695665261890399</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="11"/>
+      <c r="A14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -3665,13 +3655,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="G3:G4"/>
@@ -3687,7 +3677,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3734,7 +3724,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3752,12 +3742,12 @@
       <c r="F3" s="1">
         <v>3000</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="16">
         <v>0.954666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3773,10 +3763,10 @@
       <c r="F4" s="1">
         <v>3000</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3794,12 +3784,12 @@
       <c r="F5" s="1">
         <v>3000</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="16">
         <v>0.91566666666666596</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3815,20 +3805,20 @@
       <c r="F6" s="1">
         <v>3000</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11"/>
+      <c r="A12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3836,7 +3826,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3857,7 +3847,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B14"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3904,7 +3894,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3922,12 +3912,12 @@
       <c r="F3" s="1">
         <v>1076</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="16">
         <v>0.90799256505576198</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3943,10 +3933,10 @@
       <c r="F4" s="1">
         <v>1076</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3964,12 +3954,12 @@
       <c r="F5" s="1">
         <v>1076</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="16">
         <v>0.87546468401486899</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3985,20 +3975,20 @@
       <c r="F6" s="1">
         <v>1076</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11"/>
+      <c r="A12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -4006,7 +3996,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -4026,8 +4016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{933A4256-28A0-4E3F-90FD-B4EC800ADC32}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4076,7 +4066,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -4094,12 +4084,12 @@
       <c r="F3" s="1">
         <v>700</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="16">
         <v>0.98714285714285699</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -4115,10 +4105,10 @@
       <c r="F4" s="1">
         <v>700</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4136,12 +4126,12 @@
       <c r="F5" s="1">
         <v>700</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="16">
         <v>0.97857142857142798</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -4157,80 +4147,80 @@
       <c r="F6" s="1">
         <v>700</v>
       </c>
-      <c r="G6" s="13"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="18"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>0.94361750112764997</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>0.95394436844505204</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>0.94875283446712</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>0.96954813359528402</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>0.63689604685212298</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>0.727424749163879</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>0.67915690866510503</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>0.84461152882205504</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="11"/>
+      <c r="A14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -4238,13 +4228,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="G3:G4"/>

</xml_diff>

<commit_message>
Saving word, ppt and xlsx files.
</commit_message>
<xml_diff>
--- a/results/Comparison Summary.xlsx
+++ b/results/Comparison Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c21645ff62eb64b3/Documents/CS/CS6364/Project/query-intent-classifier/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="8_{255BB9A1-D482-4B37-8023-3EE5944DE244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D0FA7D9-FBCD-481B-B3D0-B82BBC2DD0C2}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="8_{255BB9A1-D482-4B37-8023-3EE5944DE244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41C9D69D-3E84-48C9-A08F-4AD17032E0D6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F0CFEFF8-1945-4CCF-AE0B-130C86417C10}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="44">
   <si>
     <t>precision</t>
   </si>
@@ -172,6 +172,9 @@
   <si>
     <t>IOB</t>
   </si>
+  <si>
+    <t>DIET (w/ Language Model)</t>
+  </si>
 </sst>
 </file>
 
@@ -275,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -292,6 +295,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,6 +625,86 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Overall Results'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DIET (w/ Language Model)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Overall Results'!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.94714561472421899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94430100259096506</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94376114116774301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94430100259096506</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-295E-4C97-AE5B-C62804C874B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -902,7 +991,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Overall Results'!$A$8</c:f>
+              <c:f>'Overall Results'!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -952,7 +1041,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Overall Results'!$B$7:$E$7</c:f>
+              <c:f>'Overall Results'!$B$8:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -972,7 +1061,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Overall Results'!$B$8:$E$8</c:f>
+              <c:f>'Overall Results'!$B$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1002,7 +1091,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Overall Results'!$A$9</c:f>
+              <c:f>'Overall Results'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1052,7 +1141,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Overall Results'!$B$7:$E$7</c:f>
+              <c:f>'Overall Results'!$B$8:$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1072,7 +1161,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Overall Results'!$B$9:$E$9</c:f>
+              <c:f>'Overall Results'!$B$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1094,6 +1183,86 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0D1A-48FF-9F34-ED2227ADA96D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Overall Results'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DIET (w/ Language Model)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Overall Results'!$B$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.74145193430853995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82302375359277136</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77909612623889168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90291057712991607</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-20A6-492A-AD0F-6C74C600A64D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2397,7 +2566,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2427,13 +2596,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2879,22 +3048,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7521C4CE-7B16-420F-8E5D-3BAA9CAC44AF}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -2955,78 +3127,120 @@
         <v>0.93739735517505585</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1">
+        <f>AVERAGE(BANKING77!C8,'HWU64'!C8,SNIPS!C8)</f>
+        <v>0.94714561472421899</v>
+      </c>
+      <c r="C5" s="1">
+        <f>AVERAGE(BANKING77!D8,'HWU64'!D8,SNIPS!D8)</f>
+        <v>0.94430100259096506</v>
+      </c>
+      <c r="D5" s="1">
+        <f>AVERAGE(BANKING77!E8,'HWU64'!E8,SNIPS!E8)</f>
+        <v>0.94376114116774301</v>
+      </c>
+      <c r="E5" s="1">
+        <f>AVERAGE(BANKING77!G7,'HWU64'!G7,SNIPS!G7)</f>
+        <v>0.94430100259096506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
-        <f>AVERAGE(ATIS!C10,benchmarking_data!C10,SNIPS!C10)</f>
-        <v>0.94715406626298826</v>
-      </c>
-      <c r="C8" s="1">
-        <f>AVERAGE(ATIS!D10,benchmarking_data!D10,SNIPS!D10)</f>
-        <v>0.95596265368190603</v>
-      </c>
-      <c r="D8" s="1">
-        <f>AVERAGE(ATIS!E10,benchmarking_data!E10,SNIPS!E10)</f>
-        <v>0.95153578110816106</v>
-      </c>
-      <c r="E8" s="1">
-        <f>AVERAGE(ATIS!F10,benchmarking_data!F10,SNIPS!F10)</f>
-        <v>0.97577829406396255</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <f>AVERAGE(ATIS!C12,benchmarking_data!C12,SNIPS!C12)</f>
+        <v>0.94715406626298826</v>
+      </c>
+      <c r="C9" s="1">
+        <f>AVERAGE(ATIS!D12,benchmarking_data!D12,SNIPS!D12)</f>
+        <v>0.95596265368190603</v>
+      </c>
+      <c r="D9" s="1">
+        <f>AVERAGE(ATIS!E12,benchmarking_data!E12,SNIPS!E12)</f>
+        <v>0.95153578110816106</v>
+      </c>
+      <c r="E9" s="1">
+        <f>AVERAGE(ATIS!F12,benchmarking_data!F12,SNIPS!F12)</f>
+        <v>0.97577829406396255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <f>AVERAGE(ATIS!C11,benchmarking_data!C11,SNIPS!C11)</f>
+      <c r="B10" s="1">
+        <f>AVERAGE(ATIS!C13,benchmarking_data!C13,SNIPS!C13)</f>
         <v>0.74143357608360638</v>
       </c>
-      <c r="C9" s="1">
-        <f>AVERAGE(ATIS!D11,benchmarking_data!D11,SNIPS!D11)</f>
+      <c r="C10" s="1">
+        <f>AVERAGE(ATIS!D13,benchmarking_data!D13,SNIPS!D13)</f>
         <v>0.81927246621987437</v>
       </c>
-      <c r="D9" s="1">
-        <f>AVERAGE(ATIS!E11,benchmarking_data!E11,SNIPS!E11)</f>
+      <c r="D10" s="1">
+        <f>AVERAGE(ATIS!E13,benchmarking_data!E13,SNIPS!E13)</f>
         <v>0.77742717205007639</v>
       </c>
-      <c r="E9" s="1">
-        <f>AVERAGE(ATIS!F11,benchmarking_data!F11,SNIPS!F11)</f>
+      <c r="E10" s="1">
+        <f>AVERAGE(ATIS!F13,benchmarking_data!F13,SNIPS!F13)</f>
         <v>0.90081847792143233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1">
+        <f>AVERAGE(ATIS!C14,benchmarking_data!C14,SNIPS!C14)</f>
+        <v>0.74145193430853995</v>
+      </c>
+      <c r="C11" s="1">
+        <f>AVERAGE(ATIS!D14,benchmarking_data!D14,SNIPS!D14)</f>
+        <v>0.82302375359277136</v>
+      </c>
+      <c r="D11" s="1">
+        <f>AVERAGE(ATIS!E14,benchmarking_data!E14,SNIPS!E14)</f>
+        <v>0.77909612623889168</v>
+      </c>
+      <c r="E11" s="1">
+        <f>AVERAGE(ATIS!F14,benchmarking_data!F14,SNIPS!F14)</f>
+        <v>0.90291057712991607</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3036,15 +3250,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6067AA1-4016-4948-91A0-D787ADC256B1}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G11"/>
+      <selection activeCell="B10" sqref="B10:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -3054,18 +3268,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3088,7 +3302,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3106,12 +3320,12 @@
       <c r="F3" s="1">
         <v>500</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="18">
         <v>0.97799999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3127,10 +3341,10 @@
       <c r="F4" s="1">
         <v>500</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3148,12 +3362,12 @@
       <c r="F5" s="1">
         <v>500</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="18">
         <v>0.96199999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3169,100 +3383,162 @@
       <c r="F6" s="1">
         <v>500</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.84344384822386198</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.80030345471521902</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.81719589863356601</v>
+      </c>
+      <c r="F7" s="1">
+        <v>500</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.96199999999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.96621433241491805</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.96338352142878803</v>
+      </c>
+      <c r="F8" s="1">
+        <v>500</v>
+      </c>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="1">
         <v>0.95924064768285799</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D12" s="1">
         <v>0.96408529741863003</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E12" s="1">
         <v>0.96165687097677</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F12" s="1">
         <v>0.98740854177301296</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="1">
         <v>0.93839953943580801</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D13" s="1">
         <v>0.95377413692217605</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E13" s="1">
         <v>0.94602437608821799</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F13" s="1">
         <v>0.98088725232333795</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.93459552495696996</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.95318899941486201</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.94380069524913002</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.98281606172189995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="B16" s="16"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3274,12 +3550,12 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
@@ -3287,18 +3563,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3321,7 +3597,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3339,12 +3615,12 @@
       <c r="F3" s="1">
         <v>1540</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="18">
         <v>0.88571428571428501</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3360,10 +3636,10 @@
       <c r="F4" s="1">
         <v>1540</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3381,12 +3657,12 @@
       <c r="F5" s="1">
         <v>1540</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="18">
         <v>0.90649350649350602</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3402,13 +3678,55 @@
       <c r="F6" s="1">
         <v>1540</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.93139450519886802</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.92532467532467499</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.92560479097947601</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1540</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.92532467532467499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.93139450519886802</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.92532467532467499</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.92560479097947601</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1540</v>
+      </c>
+      <c r="G8" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="16"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -3427,13 +3745,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3441,15 +3761,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A4866D-0030-4563-9E86-58AC6F214D71}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G11"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -3459,15 +3779,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -3493,7 +3813,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3511,12 +3831,12 @@
       <c r="F3" s="1">
         <v>1448</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="18">
         <v>0.99861878453038599</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3532,10 +3852,10 @@
       <c r="F4" s="1">
         <v>1448</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3553,12 +3873,12 @@
       <c r="F5" s="1">
         <v>1448</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="18">
         <v>0.98618784530386705</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3574,99 +3894,160 @@
       <c r="F6" s="1">
         <v>1448</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.98846541374169405</v>
+      </c>
+      <c r="D7">
+        <v>0.98827686414371496</v>
+      </c>
+      <c r="E7">
+        <v>0.98831059458486203</v>
+      </c>
+      <c r="F7">
+        <v>1448</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.98825966850828695</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0.98845727102695002</v>
+      </c>
+      <c r="D8">
+        <v>0.98825966850828695</v>
+      </c>
+      <c r="E8">
+        <v>0.988298156586496</v>
+      </c>
+      <c r="F8">
+        <v>1448</v>
+      </c>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.93860404997845703</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.94985829518203602</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.94419763788059297</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.97037820682359099</v>
-      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.93860404997845703</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.94985829518203602</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.94419763788059297</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.97037820682359099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="1">
         <v>0.64900514196288805</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D13" s="1">
         <v>0.77661851257356795</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E13" s="1">
         <v>0.70710023139690603</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F13" s="1">
         <v>0.87695665261890399</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.64742451154529301</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.78009630818619502</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.707595243872846</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.87597832630945205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="B17" s="16"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B8:F8"/>
+  <mergeCells count="9">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="B10:F10"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3677,12 +4058,12 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
@@ -3690,18 +4071,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3724,7 +4105,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3742,12 +4123,12 @@
       <c r="F3" s="1">
         <v>3000</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="18">
         <v>0.954666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3763,10 +4144,10 @@
       <c r="F4" s="1">
         <v>3000</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3784,12 +4165,12 @@
       <c r="F5" s="1">
         <v>3000</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="18">
         <v>0.91566666666666596</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3805,13 +4186,55 @@
       <c r="F6" s="1">
         <v>3000</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.96855030946263498</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.96633333333333304</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.96623249655426602</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.96633333333333304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.96855030946263498</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.96633333333333304</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.96623249655426602</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G8" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="16"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -3830,13 +4253,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3847,12 +4272,12 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
@@ -3860,18 +4285,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3894,7 +4319,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3912,12 +4337,12 @@
       <c r="F3" s="1">
         <v>1076</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="18">
         <v>0.90799256505576198</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3933,10 +4358,10 @@
       <c r="F4" s="1">
         <v>1076</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -3954,12 +4379,12 @@
       <c r="F5" s="1">
         <v>1076</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="18">
         <v>0.87546468401486899</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3975,13 +4400,55 @@
       <c r="F6" s="1">
         <v>1076</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.91271653857242696</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.90510765846908903</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.90548512980477902</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1076</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.92472118959107796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.92585820627480497</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.92472118959107796</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.92271749185525698</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1076</v>
+      </c>
+      <c r="G8" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="16"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -4000,13 +4467,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4014,15 +4483,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{933A4256-28A0-4E3F-90FD-B4EC800ADC32}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -4032,18 +4501,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -4066,7 +4535,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -4084,12 +4553,12 @@
       <c r="F3" s="1">
         <v>700</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="18">
         <v>0.98714285714285699</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -4105,10 +4574,10 @@
       <c r="F4" s="1">
         <v>700</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -4126,12 +4595,12 @@
       <c r="F5" s="1">
         <v>700</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="18">
         <v>0.97857142857142798</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -4147,99 +4616,160 @@
       <c r="F6" s="1">
         <v>700</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.98418413269898397</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.98285714285714199</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.98296114066849605</v>
+      </c>
+      <c r="F7" s="1">
+        <v>700</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.98285714285714199</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.98418413269898397</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.98285714285714199</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.98296114066849605</v>
+      </c>
+      <c r="F8" s="1">
+        <v>700</v>
+      </c>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.94361750112764997</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.95394436844505204</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.94875283446712</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.96954813359528402</v>
-      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.94361750112764997</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.95394436844505204</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.94875283446712</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.96954813359528402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="1">
         <v>0.63689604685212298</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D13" s="1">
         <v>0.727424749163879</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E13" s="1">
         <v>0.67915690866510503</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F13" s="1">
         <v>0.84461152882205504</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.64233576642335699</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.73578595317725703</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.68589243959469903</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.84993734335839599</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="B16" s="16"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B8:F8"/>
+  <mergeCells count="9">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="B10:F10"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>